<commit_message>
Highlighted modulation and demodulation rows :)
</commit_message>
<xml_diff>
--- a/System variables.xlsx
+++ b/System variables.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\4th Year\ELEC6023 RadCom\elec6023_assign2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23913"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -83,9 +81,6 @@
     <t>Look at 100-ish symbols to detect pilots, apply phase correction</t>
   </si>
   <si>
-    <t>Demodulation</t>
-  </si>
-  <si>
     <t>Remove pilots</t>
   </si>
   <si>
@@ -105,6 +100,9 @@
   </si>
   <si>
     <t>Henry</t>
+  </si>
+  <si>
+    <t>Complex to symbols</t>
   </si>
 </sst>
 </file>
@@ -236,7 +234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -271,7 +269,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -448,7 +446,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -459,19 +457,19 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -485,10 +483,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -499,13 +497,13 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -519,10 +517,10 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -535,11 +533,11 @@
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -551,10 +549,10 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -565,10 +563,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -579,10 +577,10 @@
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -596,10 +594,10 @@
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -610,10 +608,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -627,56 +625,61 @@
         <v>18</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added CorrectPhase.m, should be working
</commit_message>
<xml_diff>
--- a/System variables.xlsx
+++ b/System variables.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -59,7 +58,7 @@
     <t>Array of complex</t>
   </si>
   <si>
-    <t>Normalised </t>
+    <t>Normalised</t>
   </si>
   <si>
     <t>Ric</t>
@@ -101,11 +100,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -114,22 +110,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -159,7 +140,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -167,66 +148,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="5" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="20">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Good" xfId="20"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -285,32 +231,327 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D15" activeCellId="0" pane="topLeft" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.6632653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.8265306122449"/>
+    <col min="1" max="1" width="18.140625"/>
+    <col min="2" max="2" width="26.7109375"/>
+    <col min="3" max="3" width="18.5703125"/>
+    <col min="4" max="4" width="56.42578125"/>
+    <col min="5" max="1025" width="8.85546875"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -327,7 +568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -344,7 +585,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -361,7 +602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -378,7 +619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -393,7 +634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -407,7 +648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -421,7 +662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -438,7 +679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -452,7 +693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -465,11 +706,11 @@
       <c r="D11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="12">
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -483,7 +724,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -497,7 +738,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -515,12 +756,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>